<commit_message>
shiny app built, minor fixes, upgrading UI and server, new file get_data to generate .RData to be used in shiny
</commit_message>
<xml_diff>
--- a/csv/universities_after.xlsx
+++ b/csv/universities_after.xlsx
@@ -172,10 +172,10 @@
     <t xml:space="preserve">IFPB</t>
   </si>
   <si>
-    <t xml:space="preserve">-7.1355989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-34.8740557</t>
+    <t xml:space="preserve">-7.13559</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-34.87405</t>
   </si>
   <si>
     <t xml:space="preserve">Instituto Federal de Educação, Ciência e Tecnologia do Ceará</t>
@@ -196,10 +196,10 @@
     <t xml:space="preserve">IFES</t>
   </si>
   <si>
-    <t xml:space="preserve">-20.3073153</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-40.3045007</t>
+    <t xml:space="preserve">-20.30731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-40.30450</t>
   </si>
   <si>
     <t xml:space="preserve">Instituto Militar de Engenharia</t>
@@ -472,10 +472,10 @@
     <t xml:space="preserve">UNIOESTE</t>
   </si>
   <si>
-    <t xml:space="preserve">-24.9875854</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-53.451602</t>
+    <t xml:space="preserve">-24.98758</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-53.45160</t>
   </si>
   <si>
     <t xml:space="preserve">Universidade Estadual Paulista Júlio de Mesquita Filho</t>
@@ -694,10 +694,10 @@
     <t xml:space="preserve">UFSJ</t>
   </si>
   <si>
-    <t xml:space="preserve">-15.78791</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-47.8782</t>
+    <t xml:space="preserve">-20.42619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-45.06466</t>
   </si>
   <si>
     <t xml:space="preserve">Universidade Federal de São Paulo</t>
@@ -952,10 +952,10 @@
     <t xml:space="preserve">UPM</t>
   </si>
   <si>
-    <t xml:space="preserve">-23.5475011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-46.6526296</t>
+    <t xml:space="preserve">-23.54750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-46.65262</t>
   </si>
   <si>
     <t xml:space="preserve">Universidade Salvador</t>
@@ -1134,7 +1134,7 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>